<commit_message>
fill in the blank
</commit_message>
<xml_diff>
--- a/cor_treat.xlsx
+++ b/cor_treat.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,35 +360,65 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>succ</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>treat</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>C7_IND1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>emplnum</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>C7A01_01</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>C7D07_02</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>HE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>C7B01_07</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>C7D01_05</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>C7D01_05_01</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>C7D01_07</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>K_121000</t>
         </is>
@@ -399,159 +429,531 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.05744994044578157</v>
+        <v>0.428</v>
       </c>
       <c r="C2">
-        <v>0.4396894240629337</v>
+        <v>-0.093</v>
       </c>
       <c r="D2">
-        <v>-0.35873978992933</v>
+        <v>0.21</v>
       </c>
       <c r="E2">
-        <v>0.4071871561238347</v>
+        <v>-0.026</v>
       </c>
       <c r="F2">
-        <v>0.3882476896627485</v>
+        <v>0.012</v>
       </c>
       <c r="G2">
-        <v>0.243673584640089</v>
+        <v>-0.002</v>
+      </c>
+      <c r="H2">
+        <v>0.161</v>
+      </c>
+      <c r="I2">
+        <v>0.124</v>
+      </c>
+      <c r="J2">
+        <v>0.233</v>
+      </c>
+      <c r="K2">
+        <v>0.2</v>
+      </c>
+      <c r="L2">
+        <v>0.171</v>
+      </c>
+      <c r="M2">
+        <v>0.226</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>-0.05744994044578157</v>
+        <v>0.428</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>-0.05171499634299315</v>
+        <v>-0.057</v>
       </c>
       <c r="D3">
-        <v>0.03518844751709743</v>
+        <v>0.44</v>
       </c>
       <c r="E3">
-        <v>-0.110989010989011</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F3">
-        <v>0.02997281110429513</v>
+        <v>0.039</v>
       </c>
       <c r="G3">
-        <v>-0.01730117970688754</v>
+        <v>0.065</v>
+      </c>
+      <c r="H3">
+        <v>0.233</v>
+      </c>
+      <c r="I3">
+        <v>0.359</v>
+      </c>
+      <c r="J3">
+        <v>0.407</v>
+      </c>
+      <c r="K3">
+        <v>0.396</v>
+      </c>
+      <c r="L3">
+        <v>0.388</v>
+      </c>
+      <c r="M3">
+        <v>0.431</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.4396894240629337</v>
+        <v>-0.093</v>
       </c>
       <c r="B4">
-        <v>-0.05171499634299315</v>
+        <v>-0.057</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>-0.2279920077042585</v>
+        <v>-0.052</v>
       </c>
       <c r="E4">
-        <v>0.268187801588129</v>
+        <v>0.275</v>
       </c>
       <c r="F4">
-        <v>0.2269259750853674</v>
+        <v>0.256</v>
       </c>
       <c r="G4">
-        <v>0.5016234415426915</v>
+        <v>-0.042</v>
+      </c>
+      <c r="H4">
+        <v>-0.519</v>
+      </c>
+      <c r="I4">
+        <v>-0.035</v>
+      </c>
+      <c r="J4">
+        <v>-0.111</v>
+      </c>
+      <c r="K4">
+        <v>-0.101</v>
+      </c>
+      <c r="L4">
+        <v>0.03</v>
+      </c>
+      <c r="M4">
+        <v>0.057</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>-0.35873978992933</v>
+        <v>0.21</v>
       </c>
       <c r="B5">
-        <v>0.03518844751709743</v>
+        <v>0.44</v>
       </c>
       <c r="C5">
-        <v>-0.2279920077042585</v>
+        <v>-0.052</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>-0.2222759405102986</v>
+        <v>-0.127</v>
       </c>
       <c r="F5">
-        <v>-0.2975505507357798</v>
+        <v>0.094</v>
       </c>
       <c r="G5">
-        <v>-0.2169382779799844</v>
+        <v>0.19</v>
+      </c>
+      <c r="H5">
+        <v>-0.041</v>
+      </c>
+      <c r="I5">
+        <v>0.228</v>
+      </c>
+      <c r="J5">
+        <v>0.268</v>
+      </c>
+      <c r="K5">
+        <v>0.199</v>
+      </c>
+      <c r="L5">
+        <v>0.227</v>
+      </c>
+      <c r="M5">
+        <v>0.647</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>0.4071871561238347</v>
+        <v>-0.026</v>
       </c>
       <c r="B6">
-        <v>-0.110989010989011</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="C6">
-        <v>0.268187801588129</v>
+        <v>0.275</v>
       </c>
       <c r="D6">
-        <v>-0.2222759405102986</v>
+        <v>-0.127</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0.3157107840080423</v>
+        <v>0.142</v>
       </c>
       <c r="G6">
-        <v>0.1219009789699487</v>
+        <v>-0.04</v>
+      </c>
+      <c r="H6">
+        <v>0.184</v>
+      </c>
+      <c r="I6">
+        <v>0.015</v>
+      </c>
+      <c r="J6">
+        <v>0.02</v>
+      </c>
+      <c r="K6">
+        <v>-0.027</v>
+      </c>
+      <c r="L6">
+        <v>0.033</v>
+      </c>
+      <c r="M6">
+        <v>0.037</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.3882476896627485</v>
+        <v>0.012</v>
       </c>
       <c r="B7">
-        <v>0.02997281110429513</v>
+        <v>0.039</v>
       </c>
       <c r="C7">
-        <v>0.2269259750853674</v>
+        <v>0.256</v>
       </c>
       <c r="D7">
-        <v>-0.2975505507357798</v>
+        <v>0.094</v>
       </c>
       <c r="E7">
-        <v>0.3157107840080423</v>
+        <v>0.142</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0.1639391618514873</v>
+        <v>-0.04</v>
+      </c>
+      <c r="H7">
+        <v>-0.061</v>
+      </c>
+      <c r="I7">
+        <v>-0.091</v>
+      </c>
+      <c r="J7">
+        <v>-0.101</v>
+      </c>
+      <c r="K7">
+        <v>-0.09</v>
+      </c>
+      <c r="L7">
+        <v>-0.001</v>
+      </c>
+      <c r="M7">
+        <v>0.119</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.243673584640089</v>
+        <v>-0.002</v>
       </c>
       <c r="B8">
-        <v>-0.01730117970688754</v>
+        <v>0.065</v>
       </c>
       <c r="C8">
-        <v>0.5016234415426915</v>
+        <v>-0.042</v>
       </c>
       <c r="D8">
-        <v>-0.2169382779799844</v>
+        <v>0.19</v>
       </c>
       <c r="E8">
-        <v>0.1219009789699487</v>
+        <v>-0.04</v>
       </c>
       <c r="F8">
-        <v>0.1639391618514873</v>
+        <v>-0.04</v>
       </c>
       <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>-0.149</v>
+      </c>
+      <c r="I8">
+        <v>-0.03</v>
+      </c>
+      <c r="J8">
+        <v>0.142</v>
+      </c>
+      <c r="K8">
+        <v>0.048</v>
+      </c>
+      <c r="L8">
+        <v>0.089</v>
+      </c>
+      <c r="M8">
+        <v>0.065</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>0.161</v>
+      </c>
+      <c r="B9">
+        <v>0.233</v>
+      </c>
+      <c r="C9">
+        <v>-0.519</v>
+      </c>
+      <c r="D9">
+        <v>-0.041</v>
+      </c>
+      <c r="E9">
+        <v>0.184</v>
+      </c>
+      <c r="F9">
+        <v>-0.061</v>
+      </c>
+      <c r="G9">
+        <v>-0.149</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0.078</v>
+      </c>
+      <c r="J9">
+        <v>0.101</v>
+      </c>
+      <c r="K9">
+        <v>0.122</v>
+      </c>
+      <c r="L9">
+        <v>0.011</v>
+      </c>
+      <c r="M9">
+        <v>0.049</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>0.124</v>
+      </c>
+      <c r="B10">
+        <v>0.359</v>
+      </c>
+      <c r="C10">
+        <v>-0.035</v>
+      </c>
+      <c r="D10">
+        <v>0.228</v>
+      </c>
+      <c r="E10">
+        <v>0.015</v>
+      </c>
+      <c r="F10">
+        <v>-0.091</v>
+      </c>
+      <c r="G10">
+        <v>-0.03</v>
+      </c>
+      <c r="H10">
+        <v>0.078</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.222</v>
+      </c>
+      <c r="K10">
+        <v>0.245</v>
+      </c>
+      <c r="L10">
+        <v>0.298</v>
+      </c>
+      <c r="M10">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>0.233</v>
+      </c>
+      <c r="B11">
+        <v>0.407</v>
+      </c>
+      <c r="C11">
+        <v>-0.111</v>
+      </c>
+      <c r="D11">
+        <v>0.268</v>
+      </c>
+      <c r="E11">
+        <v>0.02</v>
+      </c>
+      <c r="F11">
+        <v>-0.101</v>
+      </c>
+      <c r="G11">
+        <v>0.142</v>
+      </c>
+      <c r="H11">
+        <v>0.101</v>
+      </c>
+      <c r="I11">
+        <v>0.222</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0.733</v>
+      </c>
+      <c r="L11">
+        <v>0.316</v>
+      </c>
+      <c r="M11">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>0.2</v>
+      </c>
+      <c r="B12">
+        <v>0.396</v>
+      </c>
+      <c r="C12">
+        <v>-0.101</v>
+      </c>
+      <c r="D12">
+        <v>0.199</v>
+      </c>
+      <c r="E12">
+        <v>-0.027</v>
+      </c>
+      <c r="F12">
+        <v>-0.09</v>
+      </c>
+      <c r="G12">
+        <v>0.048</v>
+      </c>
+      <c r="H12">
+        <v>0.122</v>
+      </c>
+      <c r="I12">
+        <v>0.245</v>
+      </c>
+      <c r="J12">
+        <v>0.733</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0.272</v>
+      </c>
+      <c r="M12">
+        <v>0.243</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>0.171</v>
+      </c>
+      <c r="B13">
+        <v>0.388</v>
+      </c>
+      <c r="C13">
+        <v>0.03</v>
+      </c>
+      <c r="D13">
+        <v>0.227</v>
+      </c>
+      <c r="E13">
+        <v>0.033</v>
+      </c>
+      <c r="F13">
+        <v>-0.001</v>
+      </c>
+      <c r="G13">
+        <v>0.089</v>
+      </c>
+      <c r="H13">
+        <v>0.011</v>
+      </c>
+      <c r="I13">
+        <v>0.298</v>
+      </c>
+      <c r="J13">
+        <v>0.316</v>
+      </c>
+      <c r="K13">
+        <v>0.272</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>0.226</v>
+      </c>
+      <c r="B14">
+        <v>0.431</v>
+      </c>
+      <c r="C14">
+        <v>0.057</v>
+      </c>
+      <c r="D14">
+        <v>0.647</v>
+      </c>
+      <c r="E14">
+        <v>0.037</v>
+      </c>
+      <c r="F14">
+        <v>0.119</v>
+      </c>
+      <c r="G14">
+        <v>0.065</v>
+      </c>
+      <c r="H14">
+        <v>0.049</v>
+      </c>
+      <c r="I14">
+        <v>0.249</v>
+      </c>
+      <c r="J14">
+        <v>0.308</v>
+      </c>
+      <c r="K14">
+        <v>0.243</v>
+      </c>
+      <c r="L14">
+        <v>0.251</v>
+      </c>
+      <c r="M14">
         <v>1</v>
       </c>
     </row>

</xml_diff>